<commit_message>
ADMM. Implementation of main cycle.
</commit_message>
<xml_diff>
--- a/data/HR3/Location3/Location3_2020.xlsx
+++ b/data/HR3/Location3/Location3_2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\benders-ess-planning\data\HR3\Location3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\admm-ess-planning\data\HR3\Location3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF427FD-7564-4AA9-BAD3-B433E51199D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E369704-9082-401C-BE8F-F80B50D2C6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="3540" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -10077,11 +10077,10 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1">
         <f>1/3</f>

</xml_diff>